<commit_message>
commit SPI/10 Project Management/Lab01_02_DuongMinhTam.xlsx
</commit_message>
<xml_diff>
--- a/SPI/10 Project Management/Lab01_02_DuongMinhTam.xlsx
+++ b/SPI/10 Project Management/Lab01_02_DuongMinhTam.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tam\Desktop\HK2\CNPM NÂNG CAO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tam\Desktop\bansach01\SPI\10 Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -33,12 +33,11 @@
     <definedName name="Xác_suất_rủi_ro">Ref!$C$2:$C$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="203">
   <si>
     <t>Task</t>
   </si>
@@ -682,6 +681,9 @@
   </si>
   <si>
     <t>TL hỗ trợ</t>
+  </si>
+  <si>
+    <t>checking by duong minh tam 17dh111105</t>
   </si>
 </sst>
 </file>
@@ -1484,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2610,6 +2612,11 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F54" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2656,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3533,6 +3540,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A18F03F58B8D74EA89283B2434D1156" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="234feabfce32ef1247078b7206d63e46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -3646,33 +3668,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF500F34-EDE8-4CD2-AF41-D358B22B4547}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E89793-1F2C-454B-89E0-819EEF9642BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3693,9 +3692,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08E89793-1F2C-454B-89E0-819EEF9642BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF500F34-EDE8-4CD2-AF41-D358B22B4547}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>